<commit_message>
Aggiunto input di Off da csv
</commit_message>
<xml_diff>
--- a/formats.xlsx
+++ b/formats.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sito" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Percorso" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Poi" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="QRcode" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Valori" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Valori" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,138 +24,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="115">
+  <si>
+    <t xml:space="preserve">Sito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ulsp_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provincia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toponimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microtoponimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altitudine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strade d'accesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altri elementi di localizzazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipologia sito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cronologia iniziale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cronologia finale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reperti ceramici</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reperti geologici</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reperti organici</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altri manufatti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicurezza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibilità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copertura GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copertura rete mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliografia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strumento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
   <si>
     <t xml:space="preserve"> Sito</t>
   </si>
   <si>
-    <t xml:space="preserve"> ulsp_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Titolo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Provincia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comune</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Toponimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Microtoponimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Altitudine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Strade d'accesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Altri elementi di localizzazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tipologia sito</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Definizione</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Descrizione</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cronologia iniziale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cronologia finale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reperti ceramici</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reperti geologici</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reperti organici</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Altri manufatti</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sicurezza</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Accessibilità</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Copertura GPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Copertura rete mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Foto</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bibliografia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Strumento</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ora</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Longitude</t>
-  </si>
-  <si>
     <t xml:space="preserve">44.0</t>
   </si>
   <si>
     <t xml:space="preserve">10.6</t>
   </si>
   <si>
-    <t xml:space="preserve">ulsp_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Punto d'accesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Foto accesso</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Difficoltà</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lunghezza</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Durata</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dislivello in salita</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dislivello in discesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Segnaletica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitude</t>
+    <t xml:space="preserve">Punto d'accesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foto accesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficoltà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunghezza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dislivello in salita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dislivello in discesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segnaletica</t>
   </si>
   <si>
     <t xml:space="preserve">Percorso</t>
@@ -164,22 +158,22 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> Autore</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tag primario</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Altri tag</t>
+    <t xml:space="preserve">Autore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag primario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altri tag</t>
   </si>
   <si>
     <t xml:space="preserve">POI</t>
   </si>
   <si>
-    <t xml:space="preserve"> fid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Testo</t>
+    <t xml:space="preserve">fid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testo</t>
   </si>
   <si>
     <t xml:space="preserve">QRtag</t>
@@ -188,49 +182,49 @@
     <t xml:space="preserve">Albergo</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ristorante</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parco giochi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Monumento</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parcheggio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Segnalazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fermata Bus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Frequentazione antropica</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Insediamento civile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Insediamento ecclesiastico</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Insediamento fortificato</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Infrastruttura</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Struttura devozionale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Insediamento produttivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Area funeraria</t>
+    <t xml:space="preserve">Ristorante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parco giochi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monumento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parcheggio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segnalazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fermata Bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequentazione antropica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insediamento civile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insediamento ecclesiastico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insediamento fortificato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastruttura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Struttura devozionale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insediamento produttivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area funeraria</t>
   </si>
   <si>
     <t xml:space="preserve"> ND</t>
@@ -239,109 +233,109 @@
     <t xml:space="preserve">Corpo di fabbrica</t>
   </si>
   <si>
-    <t xml:space="preserve"> Complesso architettonico composto da più corpi di fabbrica</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Struttura muraura</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Grotta</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Riparo sotto roccia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Struttura produttiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Viabilità</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elemento funzionale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elemento decorativo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elemento devozionale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elemento erratico</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Area di dispersione di materiale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Area di concentrazione di materiale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Anomalia morfologica</t>
+    <t xml:space="preserve">Complesso architettonico composto da più corpi di fabbrica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Struttura muraura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grotta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riparo sotto roccia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Struttura produttiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viabilità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemento funzionale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemento decorativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemento devozionale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemento erratico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area di dispersione di materiale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area di concentrazione di materiale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anomalia morfologica</t>
   </si>
   <si>
     <t xml:space="preserve">Preistoria (2.5 milioni-3000 anni fa)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Paleolitico (2.5 milioni-11.000 anni fa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paleolitico inferiore (2.5 milioni-120.000 anni fa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paleolitico medio (120.000-36.000 anni fa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Paleolitico superiore (36.000-11.000 anni fa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Neolitico (11.000-3500 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eneolitico (3500-2300 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Protostoria (2300-720 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età del bronzo (2300-950 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età del ferro (950-720 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Civiltà preromane (720- 89 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età romana repubblicana (509-27 a.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età romana imperiale (27 a.C.- 476 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età tardoantica (476-700 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alto medioevo (700-1000 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Basso medioevo (1000-1492 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età moderna (1492-1789 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Prima età moderna (1492-1600 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tarda età moderna (1600-1789 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età contemporanea (1789-2000 d.C.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Età subattuale (2000-oggi)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ND (Non determinata)</t>
+    <t xml:space="preserve">Paleolitico (2.5 milioni-11.000 anni fa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paleolitico inferiore (2.5 milioni-120.000 anni fa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paleolitico medio (120.000-36.000 anni fa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paleolitico superiore (36.000-11.000 anni fa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neolitico (11.000-3500 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eneolitico (3500-2300 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protostoria (2300-720 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età del bronzo (2300-950 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età del ferro (950-720 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civiltà preromane (720- 89 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età romana repubblicana (509-27 a.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età romana imperiale (27 a.C.- 476 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età tardoantica (476-700 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto medioevo (700-1000 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basso medioevo (1000-1492 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età moderna (1492-1789 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prima età moderna (1492-1600 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarda età moderna (1600-1789 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età contemporanea (1789-2000 d.C.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Età subattuale (2000-oggi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND (Non determinata)</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -353,28 +347,28 @@
     <t xml:space="preserve">Facile</t>
   </si>
   <si>
-    <t xml:space="preserve"> Media difficoltà</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Difficile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Non accessibile</t>
+    <t xml:space="preserve">Media difficoltà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non accessibile</t>
   </si>
   <si>
     <t xml:space="preserve">Completa</t>
   </si>
   <si>
-    <t xml:space="preserve"> Parziale</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Assente</t>
+    <t xml:space="preserve">Parziale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assente</t>
   </si>
   <si>
     <t xml:space="preserve">Congruente</t>
   </si>
   <si>
-    <t xml:space="preserve"> Non sufficiente</t>
+    <t xml:space="preserve">Non sufficiente</t>
   </si>
 </sst>
 </file>
@@ -389,6 +383,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -472,29 +467,29 @@
   </sheetPr>
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.27"/>
@@ -502,7 +497,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="5.04"/>
@@ -607,45 +602,45 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2" type="list">
       <formula1>Valori!A2:I2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>Valori!$A$3:$N$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2:O2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2:O2" type="list">
       <formula1>Valori!$A$4:$V$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:S2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P2:S2" type="list">
       <formula1>Valori!$A$5:$B$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U2" type="list">
       <formula1>Valori!$A$6:$D$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V2:W2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V2:W2" type="list">
       <formula1>Valori!$A$7:$C$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>
@@ -660,11 +655,11 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.12"/>
@@ -679,10 +674,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.07"/>
@@ -690,7 +685,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -744,44 +739,44 @@
         <v>28</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2" type="list">
       <formula1>Valori!$A$8:$C$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
       <formula1>Valori!$A$9:$C$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2:O2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2:O2" type="list">
       <formula1>Valori!$A$7:$C$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>
@@ -796,20 +791,20 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.73"/>
@@ -818,7 +813,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -833,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>26</v>
@@ -845,39 +840,39 @@
         <v>28</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:K2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:K2" type="list">
       <formula1>Valori!$A$1:$H$1</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>
@@ -892,25 +887,25 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -919,39 +914,39 @@
         <v>23</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>
@@ -966,243 +961,243 @@
   </sheetPr>
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="S4" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="T4" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="U4" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="V4" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPagina &amp;P</oddFooter>

</xml_diff>

<commit_message>
Sistemati tag e corretta gestione metadati
</commit_message>
<xml_diff>
--- a/formats.xlsx
+++ b/formats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sito" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="116">
   <si>
     <t xml:space="preserve">ulsp_type</t>
   </si>
@@ -176,30 +176,39 @@
     <t xml:space="preserve">QRtag</t>
   </si>
   <si>
-    <t xml:space="preserve">Albergo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ristorante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parco giochi</t>
+    <t xml:space="preserve">Grotta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ristoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accoglienza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servizi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trasporti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attrazione Naturalistica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Museo</t>
   </si>
   <si>
     <t xml:space="preserve">Monumento</t>
   </si>
   <si>
-    <t xml:space="preserve">Parcheggio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segnalazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fermata Bus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Frequentazione antropica</t>
   </si>
   <si>
@@ -234,9 +243,6 @@
   </si>
   <si>
     <t xml:space="preserve">Struttura muraura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grotta</t>
   </si>
   <si>
     <t xml:space="preserve">Riparo sotto roccia</t>
@@ -464,11 +470,11 @@
   </sheetPr>
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
@@ -656,7 +662,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.12"/>
@@ -792,7 +798,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
@@ -884,11 +890,11 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
@@ -959,10 +965,10 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.3"/>
@@ -994,201 +1000,213 @@
       <c r="H1" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>